<commit_message>
Update LBG Step Up Data Dictionary.xlsx
</commit_message>
<xml_diff>
--- a/Lloyds Bank Customer Profiling (Business Intelligence)/Data/LBG Step Up Data Dictionary.xlsx
+++ b/Lloyds Bank Customer Profiling (Business Intelligence)/Data/LBG Step Up Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://datainspirationgroup-my.sharepoint.com/personal/rachel_digdata_online/Documents/DIG/LBG/Step Up/Career challenge documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learn_DS\Git\Data Science Portfolio\Lloyds Bank Customer Profiling (Business Intelligence)\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF751FF2-B091-4AFE-BE60-6E8452CB2EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B213B9-CE01-4EDE-BDC0-63A86A8948D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Dataset" sheetId="21804" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="106">
   <si>
     <t>File Specification</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>Current Status of Loan where customers have fully paid back their loan OR did not pay back their loan, in which case they are flagged as Charged-off</t>
+  </si>
+  <si>
+    <t>Number of accounts 90 or more days past due in last 12 months</t>
   </si>
 </sst>
 </file>
@@ -816,6 +819,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="49">
@@ -2428,23 +2432,23 @@
   <dimension ref="A1:O16378"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.59765625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.69921875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.09765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.8984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.8984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="144.8984375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.09765625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.3984375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="144.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="3" customWidth="1"/>
     <col min="9" max="9" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.296875" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.09765625" style="3"/>
+    <col min="10" max="10" width="40.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
@@ -3019,7 +3023,7 @@
       </c>
       <c r="E41" s="12"/>
       <c r="F41" s="63" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="H41" s="49"/>
       <c r="K41" s="3"/>
@@ -52173,15 +52177,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095476B0E21BF1246964B10BD394B393C" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e581e7af46897015cdc83c8546e3761">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="8573de05-3fb6-496e-92d5-82c6af6150d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="889afd82ba41ef727d2fe7462b1b92d2" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -52342,6 +52337,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -52352,14 +52356,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64055B8A-09BB-4D91-9F8C-13ED6DD4AA8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63ACA3E1-28B7-40AB-8D85-9D347A96B5BA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -52378,6 +52374,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64055B8A-09BB-4D91-9F8C-13ED6DD4AA8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF064D74-C864-43C1-9272-E95844D1327E}">
   <ds:schemaRefs>

</xml_diff>